<commit_message>
updated EEG Subsidy: *Found a way to properly isolate the subsidy payment.
</commit_message>
<xml_diff>
--- a/estimates/eegSolar.xlsx
+++ b/estimates/eegSolar.xlsx
@@ -63,13 +63,13 @@
     <t>Total marginal CO2 offset, Domestic and hydro/PSP offsets only</t>
   </si>
   <si>
-    <t>denominator</t>
-  </si>
-  <si>
     <t>https://ideas.repec.org/a/eee/pubeco/v169y2019icp172-202.html</t>
   </si>
   <si>
     <t>Abrell et al. (2019) Table 5</t>
+  </si>
+  <si>
+    <t>co2_offset_per_MWh</t>
   </si>
 </sst>
 </file>
@@ -893,7 +893,7 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -956,22 +956,22 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B2">
-        <v>-175.2</v>
+        <v>-233.2</v>
       </c>
       <c r="C2">
-        <v>9.6</v>
+        <v>10.1</v>
       </c>
       <c r="J2">
         <v>1</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>13</v>
@@ -991,5 +991,6 @@
     <hyperlink ref="L2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>